<commit_message>
Commenting Code for readability
Commenting Code for readability
</commit_message>
<xml_diff>
--- a/Covid19_Texas_Data_Final.xlsx
+++ b/Covid19_Texas_Data_Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marissa\Documents\GitHub\Covid-19-Texas-Modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FB824F-9AB1-440D-9BD4-74E4510A0ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8252661-855C-433D-8085-0E8D5E9ECB24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10302" yWindow="42" windowWidth="12702" windowHeight="12006" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1092" yWindow="270" windowWidth="10848" windowHeight="12006" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid19_Texas_Data_lethality (1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Lethality_Rate</t>
-  </si>
-  <si>
-    <t>MEDIAN_AGE_TOT</t>
   </si>
   <si>
     <t>Pop_Female_Ratio</t>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Social_Distancing_Score_Rank</t>
+  </si>
+  <si>
+    <t>Median_Age</t>
   </si>
 </sst>
 </file>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -951,61 +951,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -16076,6 +16076,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16094,7 +16095,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>